<commit_message>
whole framework developed, quaternary code generating...
</commit_message>
<xml_diff>
--- a/DesignDocs/D1 四元式设计.xlsx
+++ b/DesignDocs/D1 四元式设计.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
   <si>
     <t>四元式设计</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -284,26 +284,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PROC/FUNC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BEGIN PROC/FUNC at TokenTable[Index]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>END PROC/FUNC at TokenTable[Index]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>LABEL#NUM:</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -316,14 +296,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PROC/FUNC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PARANUM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Call Procedure or Function with PARANUM parameters</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -353,6 +325,25 @@
   </si>
   <si>
     <t>RETURN DST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PROC_FUNC_INDEX</t>
+  </si>
+  <si>
+    <t>PROC_FUNC_INDEX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>END PROC/FUNC at TokenTable[PROC_FUNC_INDEX]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BEGIN PROC/FUNC at TokenTable[PROC_FUNC_INDEX]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PARA_NUM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -711,7 +702,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -719,7 +710,7 @@
     <col min="1" max="1" width="5.375" customWidth="1"/>
     <col min="2" max="2" width="14.5" customWidth="1"/>
     <col min="4" max="4" width="10.625" customWidth="1"/>
-    <col min="6" max="6" width="14.875" customWidth="1"/>
+    <col min="6" max="6" width="17.25" customWidth="1"/>
     <col min="7" max="7" width="51.25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1027,49 +1018,49 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="2"/>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="F17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G17" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="2"/>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G18" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="2"/>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G19" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -1082,14 +1073,11 @@
       <c r="C21" t="s">
         <v>4</v>
       </c>
-      <c r="D21" t="s">
-        <v>67</v>
-      </c>
       <c r="F21" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="G21" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
@@ -1100,14 +1088,11 @@
       <c r="C22" t="s">
         <v>5</v>
       </c>
-      <c r="D22" t="s">
-        <v>67</v>
-      </c>
       <c r="F22" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="G22" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
@@ -1122,7 +1107,7 @@
         <v>66</v>
       </c>
       <c r="G23" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
quaternary code generated, excepting if and for statement
</commit_message>
<xml_diff>
--- a/DesignDocs/D1 四元式设计.xlsx
+++ b/DesignDocs/D1 四元式设计.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="91">
   <si>
     <t>四元式设计</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -100,10 +100,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SRC1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -156,143 +152,198 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>DST[OFFSET]=SRC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数组元素赋值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一般元素赋值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JMP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LABEL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JMP LABEL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无条件跳转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大于则跳转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小于则跳转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>等于则跳转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不等则跳转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JNE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不大于则跳转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不小于则跳转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JNG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JNL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IF(SRC1==SRC2) JMP LABEL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IF(SRC1!=SRC2) JMP LABEL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IF(SRC1&gt;SRC2) JMP LABEL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IF(SRC1&lt;=SRC2) JMP LABEL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IF(SRC1&lt;SRC2) JMP LABEL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IF(SRC1&gt;=SRC2) JMP LABEL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>函数/过程开始</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>函数/过程结束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>标号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NUM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LABEL#NUM:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>函数/过程调用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CALL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>传递参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PROC_FUNC_INDEX</t>
+  </si>
+  <si>
+    <t>PROC_FUNC_INDEX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>END PROC/FUNC at TokenTable[PROC_FUNC_INDEX]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BEGIN PROC/FUNC at TokenTable[PROC_FUNC_INDEX]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PARA_NUM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取反</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>OFFSET</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DST[OFFSET]=SRC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数组元素赋值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一般元素赋值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JMP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LABEL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JMP LABEL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>无条件跳转</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>大于则跳转</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>小于则跳转</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>等于则跳转</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>不等则跳转</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LABEL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JNE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>不大于则跳转</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>不小于则跳转</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JNG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JNL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IF(SRC1==SRC2) JMP LABEL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IF(SRC1!=SRC2) JMP LABEL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IF(SRC1&gt;SRC2) JMP LABEL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IF(SRC1&lt;=SRC2) JMP LABEL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IF(SRC1&lt;SRC2) JMP LABEL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IF(SRC1&gt;=SRC2) JMP LABEL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>函数/过程开始</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>函数/过程结束</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>标号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LABEL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NUM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LABEL#NUM:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>函数/过程调用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CALL</t>
+    <t>DST[OFFSET]=-DST[OFFSET]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OFFSET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUSH DST[OFFSET]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RETURN DST[OFFSET]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SETP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -300,50 +351,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>传递参数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PUSHP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PUSH DST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>返回结果</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RET</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RETURN DST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PROC_FUNC_INDEX</t>
-  </si>
-  <si>
-    <t>PROC_FUNC_INDEX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>END PROC/FUNC at TokenTable[PROC_FUNC_INDEX]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BEGIN PROC/FUNC at TokenTable[PROC_FUNC_INDEX]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PARA_NUM</t>
+    <t>这里的PARA_NUM一定要有，因为后面的SETP可能不是连续的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>读语句</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>写语句</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>READ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WRITE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>READ(DST)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WRITE(DST[OFFSET])</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -699,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -726,7 +758,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -741,7 +773,7 @@
         <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -749,34 +781,31 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -785,37 +814,37 @@
         <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
@@ -827,96 +856,96 @@
         <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2"/>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="2"/>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" t="s">
         <v>39</v>
-      </c>
-      <c r="F10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="2"/>
-      <c r="B11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -925,19 +954,19 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
         <v>17</v>
@@ -946,19 +975,19 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="2"/>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
@@ -967,19 +996,19 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="2"/>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -988,19 +1017,19 @@
         <v>19</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="2"/>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
@@ -1009,125 +1038,188 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="2"/>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>82</v>
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="G17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="2"/>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>65</v>
+      </c>
+      <c r="E18" t="s">
+        <v>73</v>
       </c>
       <c r="F18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+        <v>83</v>
+      </c>
+      <c r="H18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="2"/>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" t="s">
         <v>76</v>
       </c>
-      <c r="F19" t="s">
-        <v>73</v>
-      </c>
       <c r="G19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A20" s="2"/>
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="F20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A21" s="2"/>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>82</v>
+      </c>
+      <c r="E21" t="s">
+        <v>77</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
       <c r="G21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" s="2"/>
       <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A25" s="2"/>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A26" s="2"/>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" t="s">
         <v>63</v>
       </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="2"/>
-      <c r="B23" t="s">
-        <v>64</v>
-      </c>
-      <c r="C23" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" t="s">
-        <v>66</v>
-      </c>
-      <c r="G23" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A27" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A30" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A10:A19"/>
+    <mergeCell ref="A11:A22"/>
     <mergeCell ref="B1:G1"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="A3:A9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1137,18 +1229,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="A1:XFD1048576"/>
+      <selection activeCell="C27" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.375" customWidth="1"/>
     <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="6" max="6" width="14.875" customWidth="1"/>
+    <col min="4" max="4" width="10.625" customWidth="1"/>
+    <col min="6" max="6" width="17.25" customWidth="1"/>
     <col min="7" max="7" width="51.25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1163,7 +1255,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
@@ -1178,8 +1270,8 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="2"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="2"/>
@@ -1208,10 +1300,10 @@
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" s="2"/>
     </row>
-    <row r="21" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="22" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.15">
@@ -1227,14 +1319,17 @@
       <c r="A26" s="2"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A27" s="1"/>
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A28" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:G1"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A10:A19"/>
-    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="A11:A20"/>
+    <mergeCell ref="A22:A27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>